<commit_message>
pipeline variables excel finished
</commit_message>
<xml_diff>
--- a/doc/pipeline-variables.xlsx
+++ b/doc/pipeline-variables.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20366"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0D6C670-94A7-4878-8DC2-E565D1CA709B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,9 +19,90 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+  <si>
+    <t>ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FI</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>EX</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MEM</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>WB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pc</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>inst</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>regwe</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>alusel</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>cb</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>cf</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>memlen</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>memwe</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>rd1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>rd2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>rt</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>rd</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>aluout</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>memrd</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +110,55 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,15 +166,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="输出" xfId="1" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -330,13 +474,146 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="9.06640625" style="1"/>
+    <col min="2" max="2" width="8.9296875" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.06640625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
middle layer gen ok
</commit_message>
<xml_diff>
--- a/doc/pipeline-variables.xlsx
+++ b/doc/pipeline-variables.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20366"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0D6C670-94A7-4878-8DC2-E565D1CA709B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE4D3D6-48E8-43CB-AEF0-1452E512545B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -95,6 +95,14 @@
   </si>
   <si>
     <t>memrd</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>inst</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>width</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -102,6 +110,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="0.00_);[Red]\(0.00\)"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -127,7 +138,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -141,19 +152,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="-0.249977111117893"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -188,12 +187,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -475,141 +477,295 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.06640625" style="1"/>
-    <col min="2" max="2" width="8.9296875" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.06640625" style="1"/>
+    <col min="1" max="2" width="9.06640625" style="1"/>
+    <col min="3" max="3" width="8.9296875" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B2" s="2">
+        <v>32</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B3" s="2">
+        <v>32</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
       <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="3"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="3">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B6" s="2">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B7" s="2">
+        <v>4</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="3">
+        <v>1</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B8" s="2">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="3">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B9" s="2">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="3">
+        <v>1</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1</v>
+      </c>
+      <c r="F9" s="3">
+        <v>1</v>
+      </c>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B10" s="2">
+        <v>32</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="3">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B11" s="2">
+        <v>32</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="3">
+        <v>1</v>
+      </c>
+      <c r="E11" s="3">
+        <v>1</v>
+      </c>
+      <c r="F11" s="3">
+        <v>1</v>
+      </c>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B12" s="2">
+        <v>5</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="3">
+        <v>1</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1</v>
+      </c>
+      <c r="F12" s="3">
+        <v>1</v>
+      </c>
+      <c r="G12" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B13" s="2">
+        <v>5</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="3">
+        <v>1</v>
+      </c>
+      <c r="E13" s="3">
+        <v>1</v>
+      </c>
+      <c r="F13" s="3">
+        <v>1</v>
+      </c>
+      <c r="G13" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B14" s="2">
+        <v>32</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="3">
+        <v>1</v>
+      </c>
+      <c r="F14" s="3">
+        <v>1</v>
+      </c>
+      <c r="G14" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
+      <c r="B15" s="2">
+        <v>32</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="3">
+        <v>1</v>
+      </c>
+      <c r="G15" s="3">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
lw slot to be dealt
</commit_message>
<xml_diff>
--- a/doc/pipeline-variables.xlsx
+++ b/doc/pipeline-variables.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20366"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C26F5B2-458B-4CC4-BE91-26B355F60DEE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3CA4575-CEF3-4268-9073-8EAC5F704148}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -491,7 +491,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -692,7 +692,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1">

</xml_diff>